<commit_message>
aggiornato excel, tolti commenti non più utili
</commit_message>
<xml_diff>
--- a/docs/excel/Tracciamento Sviluppo.xlsx
+++ b/docs/excel/Tracciamento Sviluppo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ugo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ugo\source\repos\UgoEngine\docs\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAFB0F7-8854-494B-A35A-D4EA25054CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35A54E9-D993-42E6-93B8-8B44E2E6A515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
   <si>
     <t xml:space="preserve">   </t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>Dati</t>
-  </si>
-  <si>
-    <t>Stati</t>
   </si>
   <si>
     <t>Da pianificare; Da implementare; In sviluppo; Funzionale; Completato; In revisione;</t>
@@ -264,6 +261,31 @@
   </si>
   <si>
     <t>ColliderSystem</t>
+  </si>
+  <si>
+    <t>EntityFactory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crea entità con componenti predefiniti in modo modulare e riutilizzabile </t>
+  </si>
+  <si>
+    <t>es. createPLayer(), createEnemy(), createTree()</t>
+  </si>
+  <si>
+    <t>AnimationSystem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aggiorna lo sprite del renderComponent in base a tempo trascorso e un machine state
+</t>
+  </si>
+  <si>
+    <t>DeltaTime</t>
+  </si>
+  <si>
+    <t>Traccia il tempo trascorso, utile per disaccoppiare Fisica e Animazioni dal frame rate</t>
+  </si>
+  <si>
+    <t>STATI</t>
   </si>
 </sst>
 </file>
@@ -1015,21 +1037,6 @@
   </cellStyles>
   <dxfs count="38">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1325,10 +1332,18 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color rgb="FF404040"/>
-        </bottom>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1365,6 +1380,13 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color rgb="FF404040"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1979,7 +2001,7 @@
     <tableColumn id="9" xr3:uid="{A3C4835A-9487-4663-AFA6-4CD283A07B70}" name="Colonna8" dataDxfId="25"/>
     <tableColumn id="10" xr3:uid="{DCED20B1-F0B5-43B9-B90B-82FF44283B54}" name="Colonna9" dataDxfId="24"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1996,40 +2018,40 @@
     <tableColumn id="5" xr3:uid="{2995F736-B54F-4027-86D3-DD1AB1ABA13F}" name="Note" dataDxfId="15"/>
     <tableColumn id="6" xr3:uid="{8DF335C5-2776-4643-A5E7-02D3EB9B6E03}" name="Stato" dataDxfId="14"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A6390330-E18D-4D3A-9EB6-B2745F72EFC6}" name="Tabella4" displayName="Tabella4" ref="I2:K6" totalsRowShown="0">
-  <autoFilter ref="I2:K6" xr:uid="{A6390330-E18D-4D3A-9EB6-B2745F72EFC6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A6390330-E18D-4D3A-9EB6-B2745F72EFC6}" name="Tabella4" displayName="Tabella4" ref="I2:K12" totalsRowShown="0">
+  <autoFilter ref="I2:K12" xr:uid="{A6390330-E18D-4D3A-9EB6-B2745F72EFC6}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0A7ECEFC-B5F2-4024-9A31-B23091CF35C1}" name="Tags"/>
     <tableColumn id="2" xr3:uid="{EE055E41-BFE7-427E-8856-6D89EE96F520}" name="File"/>
     <tableColumn id="3" xr3:uid="{4C6D62A7-7DE3-4717-8986-67860DA5A1C4}" name="Note"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{92EFF6A5-4299-411B-8A94-3AB8507524C8}" name="Tabella1342" displayName="Tabella1342" ref="B2:K12" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" headerRowCellStyle="Titolo 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{92EFF6A5-4299-411B-8A94-3AB8507524C8}" name="Tabella1342" displayName="Tabella1342" ref="B2:K12" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" headerRowCellStyle="Titolo 1">
   <autoFilter ref="B2:K12" xr:uid="{F2AF0F4D-D3DE-4B3C-A3FC-AC365AA49C6A}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{817A9355-6F8B-492E-AD30-81DDC3D6F855}" name="Utility" dataDxfId="0" dataCellStyle="Titolo 3">
+    <tableColumn id="1" xr3:uid="{817A9355-6F8B-492E-AD30-81DDC3D6F855}" name="Utility" dataDxfId="9" dataCellStyle="Titolo 3">
       <calculatedColumnFormula>_xlfn.CONCAT("UTILS",TEXT(ROW()-ROW($A$2)-1,"000"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{73510014-F400-4E01-9306-DFBE23B9491B}" name="Nome" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{B59CA529-38D0-440A-A410-F0943D8628DF}" name="File" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{33445314-575F-441E-9B56-0995040C4AA3}" name="Responsabilità" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{87C880EB-E8EE-4EC0-AE08-914F712BE1AA}" name="Note" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{8D957D05-E582-4ACD-8CF0-C631DEF04713}" name="Stato" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{5A4F8278-13B4-4361-A496-B13E25B522DE}" name="Components" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{5F303927-975B-4598-8E7B-4A3188A5E33E}" name="Colonna7" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{62401049-C5A2-4DBB-83C7-C527BFA6099F}" name="Colonna8" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{1F8B501F-BDBE-4460-A5A4-03F12E9C4291}" name="Colonna9" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{73510014-F400-4E01-9306-DFBE23B9491B}" name="Nome" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{B59CA529-38D0-440A-A410-F0943D8628DF}" name="File" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{33445314-575F-441E-9B56-0995040C4AA3}" name="Responsabilità" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{87C880EB-E8EE-4EC0-AE08-914F712BE1AA}" name="Note" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{8D957D05-E582-4ACD-8CF0-C631DEF04713}" name="Stato" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{5A4F8278-13B4-4361-A496-B13E25B522DE}" name="Components" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{5F303927-975B-4598-8E7B-4A3188A5E33E}" name="Colonna7" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{62401049-C5A2-4DBB-83C7-C527BFA6099F}" name="Colonna8" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{1F8B501F-BDBE-4460-A5A4-03F12E9C4291}" name="Colonna9" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2327,7 +2349,7 @@
   <dimension ref="B1:K12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2392,7 +2414,7 @@
     </row>
     <row r="4" spans="2:11" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="str">
-        <f t="shared" ref="B4:B12" si="0">_xlfn.CONCAT("SYS",TEXT(ROW()-ROW($A$2)-1,"000"))</f>
+        <f>_xlfn.CONCAT("SYS",TEXT(ROW()-ROW($A$2)-1,"000"))</f>
         <v>SYS001</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2415,7 +2437,7 @@
     </row>
     <row r="5" spans="2:11" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B4:B12" si="0">_xlfn.CONCAT("SYS",TEXT(ROW()-ROW($A$2)-1,"000"))</f>
         <v>SYS002</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -2430,7 +2452,7 @@
         <v>19</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -2442,20 +2464,20 @@
         <v>SYS003</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3" t="s">
@@ -2469,22 +2491,22 @@
         <v>SYS004</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>0</v>
@@ -2498,13 +2520,13 @@
         <v>SYS005</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -2516,11 +2538,17 @@
         <f t="shared" si="0"/>
         <v>SYS006</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -2609,7 +2637,7 @@
   <dimension ref="B1:K12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2648,7 +2676,7 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J2" t="s">
         <v>7</v>
@@ -2680,17 +2708,17 @@
         <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" t="s">
         <v>51</v>
-      </c>
-      <c r="J4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -2699,13 +2727,13 @@
         <v>COM002</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
@@ -2718,36 +2746,36 @@
         <v>COM003</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f t="shared" si="0"/>
         <v>COM004</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -2756,17 +2784,17 @@
         <v>COM005</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -2844,8 +2872,8 @@
   </sheetPr>
   <dimension ref="B1:K12"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2866,7 +2894,7 @@
     <row r="1" spans="2:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>3</v>
@@ -2910,23 +2938,23 @@
     </row>
     <row r="4" spans="2:11" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="str">
-        <f t="shared" ref="B3:B12" si="0">_xlfn.CONCAT("UTILS",TEXT(ROW()-ROW($A$2)-1,"000"))</f>
+        <f t="shared" ref="B4:B12" si="0">_xlfn.CONCAT("UTILS",TEXT(ROW()-ROW($A$2)-1,"000"))</f>
         <v>UTILS001</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -2939,15 +2967,15 @@
         <v>UTILS002</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -2960,15 +2988,15 @@
         <v>UTILS003</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -2982,11 +3010,19 @@
         <f t="shared" si="0"/>
         <v>UTILS004</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
         <v>0</v>
@@ -2999,11 +3035,17 @@
         <f t="shared" si="0"/>
         <v>UTILS005</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -3103,27 +3145,30 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="93.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-    </row>
+    <row r="3" spans="1:2" ht="63.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>